<commit_message>
izzy's poets, round 1
</commit_message>
<xml_diff>
--- a/sql/genres.xlsx
+++ b/sql/genres.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="poet lookup" sheetId="2" r:id="rId2"/>
+    <sheet name="genre lookup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="183">
   <si>
     <t>poetid</t>
   </si>
@@ -175,9 +176,6 @@
     <t>Xenokrates</t>
   </si>
   <si>
-    <t>Iambs</t>
-  </si>
-  <si>
     <t>-es</t>
   </si>
   <si>
@@ -223,9 +221,6 @@
     <t>Euangelos</t>
   </si>
   <si>
-    <t>Eumelos</t>
-  </si>
-  <si>
     <t>Euneidai</t>
   </si>
   <si>
@@ -329,6 +324,255 @@
   </si>
   <si>
     <t>Iambos</t>
+  </si>
+  <si>
+    <t>Skolia</t>
+  </si>
+  <si>
+    <t>Alcaeus</t>
+  </si>
+  <si>
+    <t>Alcman</t>
+  </si>
+  <si>
+    <t>Anacreon</t>
+  </si>
+  <si>
+    <t>Ananius</t>
+  </si>
+  <si>
+    <t>Apollodorus</t>
+  </si>
+  <si>
+    <t>Archilochus</t>
+  </si>
+  <si>
+    <t>Arion</t>
+  </si>
+  <si>
+    <t>Asius</t>
+  </si>
+  <si>
+    <t>Bacchylides</t>
+  </si>
+  <si>
+    <t>Callinus</t>
+  </si>
+  <si>
+    <t>Cedeides</t>
+  </si>
+  <si>
+    <t>Charixena</t>
+  </si>
+  <si>
+    <t>Corinna</t>
+  </si>
+  <si>
+    <t>Critias</t>
+  </si>
+  <si>
+    <t>Cydias</t>
+  </si>
+  <si>
+    <t>Demodocus</t>
+  </si>
+  <si>
+    <t>Dionysius Chalkus</t>
+  </si>
+  <si>
+    <t>Echembrotus</t>
+  </si>
+  <si>
+    <t>Eunicus</t>
+  </si>
+  <si>
+    <t>Euripides</t>
+  </si>
+  <si>
+    <t>Hermippus</t>
+  </si>
+  <si>
+    <t>Hipponax</t>
+  </si>
+  <si>
+    <t>Ibycus</t>
+  </si>
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>Lamprocles</t>
+  </si>
+  <si>
+    <t>Lamprus</t>
+  </si>
+  <si>
+    <t>Lasus</t>
+  </si>
+  <si>
+    <t>Mimnermus</t>
+  </si>
+  <si>
+    <t>Myrtis</t>
+  </si>
+  <si>
+    <t>Olympus</t>
+  </si>
+  <si>
+    <t>Panarces</t>
+  </si>
+  <si>
+    <t>Philiadas</t>
+  </si>
+  <si>
+    <t>Phocylides</t>
+  </si>
+  <si>
+    <t>Polymnestus</t>
+  </si>
+  <si>
+    <t>Pratinas</t>
+  </si>
+  <si>
+    <t>Sacadas</t>
+  </si>
+  <si>
+    <t>Sappho</t>
+  </si>
+  <si>
+    <t>Scythinus</t>
+  </si>
+  <si>
+    <t>Semonides</t>
+  </si>
+  <si>
+    <t>Simonides</t>
+  </si>
+  <si>
+    <t>Solon</t>
+  </si>
+  <si>
+    <t>Sophocles</t>
+  </si>
+  <si>
+    <t>Stesichorus</t>
+  </si>
+  <si>
+    <t>Susarion</t>
+  </si>
+  <si>
+    <t>Terpander</t>
+  </si>
+  <si>
+    <t>Theognis</t>
+  </si>
+  <si>
+    <t>Timocreon</t>
+  </si>
+  <si>
+    <t>Tyrtaeus</t>
+  </si>
+  <si>
+    <t>Tynnichus</t>
+  </si>
+  <si>
+    <t>Xanthus</t>
+  </si>
+  <si>
+    <t>Eumelos #2</t>
+  </si>
+  <si>
+    <t>Eumelos #1</t>
+  </si>
+  <si>
+    <t>Thaletas</t>
+  </si>
+  <si>
+    <t>Xenophanes</t>
+  </si>
+  <si>
+    <t>Partheneion</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Choral Dance</t>
+  </si>
+  <si>
+    <t>Satyr</t>
+  </si>
+  <si>
+    <t>what does this mean?</t>
+  </si>
+  <si>
+    <t>Hypochrematon</t>
+  </si>
+  <si>
+    <t>Epinician</t>
+  </si>
+  <si>
+    <t>(Epic = Anacreonta?)</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Lament (epikedeion?)</t>
+  </si>
+  <si>
+    <t>Komos</t>
+  </si>
+  <si>
+    <t>(see Beazley ARV i 31)</t>
+  </si>
+  <si>
+    <t>Prose</t>
+  </si>
+  <si>
+    <t>Eulogy</t>
+  </si>
+  <si>
+    <t>Lament (Dirge)</t>
+  </si>
+  <si>
+    <t>Laws?</t>
+  </si>
+  <si>
+    <t>Tragedy</t>
+  </si>
+  <si>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>Enoplion</t>
+  </si>
+  <si>
+    <t>Parody</t>
+  </si>
+  <si>
+    <t>(Silloi = "Lampoons"?)</t>
+  </si>
+  <si>
+    <t>Epode</t>
+  </si>
+  <si>
+    <t>Lament</t>
+  </si>
+  <si>
+    <t>Psogon</t>
+  </si>
+  <si>
+    <t>Polemisterion</t>
+  </si>
+  <si>
+    <t>"Lyric"</t>
+  </si>
+  <si>
+    <t>"Melos"</t>
   </si>
 </sst>
 </file>
@@ -389,9 +633,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,10 +717,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="70">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -443,6 +735,29 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -454,6 +769,29 @@
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,16 +1070,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="44.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -759,9 +1097,12 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>156</v>
+      </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="28">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -817,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -839,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7">
         <v>11</v>
@@ -887,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -909,13 +1250,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -953,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -968,14 +1309,14 @@
         <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <v>11</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="28">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -990,7 +1331,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="28">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1037,7 +1378,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="6">
         <v>62</v>
@@ -1058,7 +1399,7 @@
         <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D22">
         <v>11</v>
@@ -1088,13 +1429,13 @@
         <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1451,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26">
         <v>55</v>
@@ -1124,7 +1465,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>55</v>
@@ -1138,7 +1479,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28">
         <v>55</v>
@@ -1152,7 +1493,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29">
         <v>55</v>
@@ -1164,7 +1505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1178,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1214,13 +1555,13 @@
         <v>77</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D33">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1234,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1276,7 +1617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -1290,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="28">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
@@ -1312,13 +1653,13 @@
         <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D40">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -1340,13 +1681,13 @@
         <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D42">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -1368,7 +1709,7 @@
         <v>24</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D44">
         <v>11</v>
@@ -1376,13 +1717,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B45">
         <v>25</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45">
         <v>11</v>
@@ -1424,13 +1765,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D48">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28">
+    <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
@@ -1473,33 +1814,32 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52">
+        <v>83</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>2</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53">
-        <v>84</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D53">
-        <v>11</v>
-      </c>
-      <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
@@ -1509,40 +1849,40 @@
         <v>84</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55">
+        <v>84</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>85</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>3</v>
-      </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" ht="28">
-      <c r="A56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
       </c>
       <c r="F56" s="3"/>
     </row>
@@ -1554,29 +1894,29 @@
         <v>7</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="D57">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" ht="28">
+    <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -1584,10 +1924,10 @@
         <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" s="3"/>
     </row>
@@ -1599,10 +1939,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F60" s="3"/>
     </row>
@@ -1614,10 +1954,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F61" s="3"/>
     </row>
@@ -1629,14 +1969,14 @@
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D62">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" ht="28">
+    <row r="63" spans="1:6">
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
@@ -1644,60 +1984,1910 @@
         <v>6</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63">
+        <v>7</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>9</v>
       </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="4" t="s">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>90</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D64">
+      <c r="D65">
         <v>3</v>
       </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="6:6">
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="6:6">
+    <row r="66" spans="1:6">
+      <c r="A66" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B66">
+        <f>VLOOKUP(A66,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="6:6">
+    <row r="67" spans="1:6">
+      <c r="A67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67">
+        <f>VLOOKUP(A67,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67">
+        <v>13</v>
+      </c>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="6:6">
+    <row r="68" spans="1:6">
+      <c r="A68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68">
+        <f>VLOOKUP(A68,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="6:6">
+    <row r="69" spans="1:6">
+      <c r="A69" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69">
+        <f>VLOOKUP(A69,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="6:6">
+    <row r="70" spans="1:6">
+      <c r="A70" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70">
+        <f>VLOOKUP(A70,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="6:6">
+    <row r="71" spans="1:6">
+      <c r="A71" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71">
+        <f>VLOOKUP(A71,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71">
+        <v>11</v>
+      </c>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="6:6">
+    <row r="72" spans="1:6">
+      <c r="A72" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72">
+        <f>VLOOKUP(A72,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72">
+        <v>11</v>
+      </c>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="6:6">
+    <row r="73" spans="1:6">
+      <c r="A73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73">
+        <f>VLOOKUP(A73,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <v>6</v>
+      </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="6:6">
+    <row r="74" spans="1:6">
+      <c r="A74" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74">
+        <f>VLOOKUP(A74,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="6:6">
+    <row r="75" spans="1:6">
+      <c r="A75" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75">
+        <f>VLOOKUP(A75,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75">
+        <v>11</v>
+      </c>
       <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76">
+        <f>VLOOKUP(A76,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77">
+        <f>VLOOKUP(A77,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77">
+        <v>9</v>
+      </c>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78">
+        <f>VLOOKUP(A78,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
+        <v>160</v>
+      </c>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79">
+        <f>VLOOKUP(A79,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80">
+        <f>VLOOKUP(A80,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81">
+        <f>VLOOKUP(A81,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D81">
+        <v>21</v>
+      </c>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B82">
+        <f>VLOOKUP(A82,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82">
+        <v>7</v>
+      </c>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83">
+        <f>VLOOKUP(A83,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>99</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D83">
+        <v>15</v>
+      </c>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B84">
+        <v>99</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85">
+        <f>VLOOKUP(A85,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D85">
+        <v>16</v>
+      </c>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86">
+        <f>VLOOKUP(A86,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87">
+        <f>VLOOKUP(A87,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87">
+        <v>6</v>
+      </c>
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B88">
+        <f>VLOOKUP(A88,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88">
+        <v>8</v>
+      </c>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89">
+        <f>VLOOKUP(A89,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89">
+        <v>10</v>
+      </c>
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90">
+        <f>VLOOKUP(A90,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D90">
+        <v>13</v>
+      </c>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91">
+        <f>VLOOKUP(A91,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D91">
+        <v>22</v>
+      </c>
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92">
+        <f>VLOOKUP(A92,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92">
+        <v>4</v>
+      </c>
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B93">
+        <f>VLOOKUP(A93,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D93">
+        <v>12</v>
+      </c>
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B94">
+        <f>VLOOKUP(A94,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>101</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95">
+        <f>VLOOKUP(A95,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>102</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96">
+        <f>VLOOKUP(A96,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>104</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97">
+        <f>VLOOKUP(A97,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>104</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98">
+        <f>VLOOKUP(A98,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>105</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D98">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99">
+        <f>VLOOKUP(A99,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>105</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B100">
+        <f>VLOOKUP(A100,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>105</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B101">
+        <f>VLOOKUP(A101,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>106</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D101">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102">
+        <f>VLOOKUP(A102,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>107</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103">
+        <f>VLOOKUP(A103,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>107</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104">
+        <f>VLOOKUP(A104,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105">
+        <f>VLOOKUP(A105,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106">
+        <f>VLOOKUP(A106,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>109</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107">
+        <f>VLOOKUP(A107,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>111</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B108">
+        <f>VLOOKUP(A108,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>112</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109">
+        <f>VLOOKUP(A109,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>112</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D109">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="6" customFormat="1">
+      <c r="A110" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" s="6">
+        <f>VLOOKUP(A110,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>113</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111">
+        <f>VLOOKUP(A111,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>114</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D111">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112">
+        <f>VLOOKUP(A112,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>114</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B113">
+        <f>VLOOKUP(A113,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>114</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D113">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114">
+        <f>VLOOKUP(A114,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>114</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B115">
+        <f>VLOOKUP(A115,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>115</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116">
+        <f>VLOOKUP(A116,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>115</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D116">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B117">
+        <f>VLOOKUP(A117,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>116</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D117">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118">
+        <f>VLOOKUP(A118,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>116</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D118">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B119">
+        <f>VLOOKUP(A119,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>116</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D119">
+        <v>19</v>
+      </c>
+      <c r="E119" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B120">
+        <f>VLOOKUP(A120,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D120">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B121">
+        <f>VLOOKUP(A121,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D121">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122">
+        <f>VLOOKUP(A122,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123">
+        <f>VLOOKUP(A123,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124">
+        <f>VLOOKUP(A124,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D124">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <f>VLOOKUP(A125,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <f>VLOOKUP(A126,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D126">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B127">
+        <f>VLOOKUP(A127,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B128">
+        <f>VLOOKUP(A128,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D128">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B129">
+        <f>VLOOKUP(A129,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>118</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B130">
+        <f>VLOOKUP(A130,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>119</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B131">
+        <f>VLOOKUP(A131,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>119</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D131">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B132">
+        <f>VLOOKUP(A132,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>121</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B133">
+        <f>VLOOKUP(A133,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>122</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B134">
+        <f>VLOOKUP(A134,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>122</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D134">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B135">
+        <f>VLOOKUP(A135,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>124</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D135">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B136">
+        <f>VLOOKUP(A136,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>124</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B137">
+        <f>VLOOKUP(A137,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>126</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B138">
+        <f>VLOOKUP(A138,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>127</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D138">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B139">
+        <f>VLOOKUP(A139,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>127</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140">
+        <f>VLOOKUP(A140,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>128</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B141">
+        <f>VLOOKUP(A141,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>128</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D141">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B142">
+        <f>VLOOKUP(A142,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>129</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D142">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B143">
+        <f>VLOOKUP(A143,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>129</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D143">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B144">
+        <f>VLOOKUP(A144,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>131</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B145">
+        <f>VLOOKUP(A145,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>131</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B146">
+        <f>VLOOKUP(A146,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>132</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147">
+        <f>VLOOKUP(A147,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>132</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D147">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B148">
+        <f>VLOOKUP(A148,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>132</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B149">
+        <f>VLOOKUP(A149,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>133</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D149">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150">
+        <f>VLOOKUP(A150,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>134</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B151">
+        <f>VLOOKUP(A151,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>134</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D151">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B152">
+        <f>VLOOKUP(A152,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D152">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B153">
+        <f>VLOOKUP(A153,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D153">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B154">
+        <f>VLOOKUP(A154,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B155">
+        <f>VLOOKUP(A155,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D155">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B156">
+        <f>VLOOKUP(A156,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D156">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B157">
+        <f>VLOOKUP(A157,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D157">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B158">
+        <f>VLOOKUP(A158,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D158">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B159">
+        <f>VLOOKUP(A159,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>135</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D159">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B160">
+        <f>VLOOKUP(A160,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>136</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B161">
+        <f>VLOOKUP(A161,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>136</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D161">
+        <v>15</v>
+      </c>
+      <c r="E161" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B162">
+        <f>VLOOKUP(A162,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>136</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D162">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B163">
+        <f>VLOOKUP(A163,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>137</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B164">
+        <f>VLOOKUP(A164,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>137</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D164">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B165">
+        <f>VLOOKUP(A165,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>137</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D165">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B166">
+        <f>VLOOKUP(A166,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>138</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B167">
+        <f>VLOOKUP(A167,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>138</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D167">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B168">
+        <f>VLOOKUP(A168,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>139</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D168">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B169">
+        <f>VLOOKUP(A169,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>139</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D169">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B170">
+        <f>VLOOKUP(A170,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D170">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B171">
+        <f>VLOOKUP(A171,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>141</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D171">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B172">
+        <f>VLOOKUP(A172,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>141</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D172">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B173">
+        <f>VLOOKUP(A173,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>142</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D173">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B174">
+        <f>VLOOKUP(A174,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>142</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D174">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B175">
+        <f>VLOOKUP(A175,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>143</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B176">
+        <f>VLOOKUP(A176,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>144</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D176">
+        <v>27</v>
+      </c>
+      <c r="E176" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B177">
+        <f>VLOOKUP(A177,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>144</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D177">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B178">
+        <f>VLOOKUP(A178,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>144</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D178">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B179">
+        <f>VLOOKUP(A179,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>145</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B180">
+        <f>VLOOKUP(A180,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>145</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D180">
+        <v>28</v>
+      </c>
+      <c r="E180" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B181">
+        <f>VLOOKUP(A181,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>145</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D181">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B182">
+        <f>VLOOKUP(A182,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>146</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D182">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B183">
+        <f>VLOOKUP(A183,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>148</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D183">
+        <v>15</v>
+      </c>
+      <c r="E183" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B184">
+        <f>VLOOKUP(A184,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>148</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B185">
+        <f>VLOOKUP(A185,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>148</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D185">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B186">
+        <f>VLOOKUP(A186,'poet lookup'!$A$1:$B$137,2,FALSE)</f>
+        <v>148</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D186">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:D58">
@@ -1715,775 +3905,1108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection sqref="A1:B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3"/>
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="3">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="3">
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="3">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="3">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" s="3">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="B21" s="3">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B24" s="3">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B25" s="3">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="B26" s="3">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="B28" s="3">
-        <v>33</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B29" s="3">
-        <v>58</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B30" s="3">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="B31" s="3">
-        <v>27</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="B32" s="3">
-        <v>41</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B33" s="3">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="B34" s="3">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B37" s="3">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B38" s="3">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="B39" s="3">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B40" s="3">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3">
-        <v>65</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="B43" s="3">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B44" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B45" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B46" s="3">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="B47" s="3">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="B48" s="3">
-        <v>69</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B49" s="3">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="B50" s="3">
-        <v>71</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="B51" s="3">
-        <v>55</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B52" s="3">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B53" s="3">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B54" s="3">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B56" s="3">
-        <v>51</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="B57" s="3">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B58" s="3">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B59" s="3">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="B60" s="3">
-        <v>46</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3">
-        <v>20</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="B62" s="3">
-        <v>47</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B63" s="3">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B64" s="3">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B65" s="3">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B66" s="3">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B67" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="8" t="s">
-        <v>85</v>
+      <c r="A68" t="s">
+        <v>76</v>
       </c>
       <c r="B68" s="3">
-        <v>91</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="B69" s="3">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B70" s="3">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="B71" s="3">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B72" s="3">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="B73" s="3">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B74" s="3">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B75" s="3">
-        <v>78</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="4" t="s">
-        <v>91</v>
+      <c r="A76" t="s">
+        <v>126</v>
       </c>
       <c r="B76" s="3">
-        <v>79</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B77" s="3">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="4" t="s">
-        <v>92</v>
+      <c r="A78" t="s">
+        <v>127</v>
       </c>
       <c r="B78" s="3">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B79" s="3">
-        <v>24</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="B80" s="3">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="4" t="s">
-        <v>45</v>
+      <c r="A81" t="s">
+        <v>82</v>
       </c>
       <c r="B81" s="3">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B82" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="4" t="s">
-        <v>94</v>
+      <c r="A83" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B83" s="3">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B84" s="3">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="4" t="s">
-        <v>46</v>
+      <c r="A85" t="s">
+        <v>85</v>
       </c>
       <c r="B85" s="3">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="B86" s="3">
-        <v>2</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="4" t="s">
-        <v>47</v>
+      <c r="A87" t="s">
+        <v>86</v>
       </c>
       <c r="B87" s="3">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="4" t="s">
-        <v>48</v>
+      <c r="A88" t="s">
+        <v>129</v>
       </c>
       <c r="B88" s="3">
-        <v>85</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="4" t="s">
-        <v>95</v>
+      <c r="A89" t="s">
+        <v>17</v>
       </c>
       <c r="B89" s="3">
-        <v>86</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="B90" s="3">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B91" s="3">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B92" s="3">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="4" t="s">
-        <v>98</v>
+      <c r="A93" t="s">
+        <v>130</v>
       </c>
       <c r="B93" s="3">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="B94" s="3">
-        <v>45</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B95" s="3">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B96" s="3">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>132</v>
+      </c>
+      <c r="B98" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>133</v>
+      </c>
+      <c r="B101" s="3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B102" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B104" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>22</v>
+      </c>
+      <c r="B105" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" s="3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>136</v>
+      </c>
+      <c r="B110" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>137</v>
+      </c>
+      <c r="B111" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>138</v>
+      </c>
+      <c r="B112" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>139</v>
+      </c>
+      <c r="B113" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>140</v>
+      </c>
+      <c r="B114" s="3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B115" s="3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+      <c r="B117" s="3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B118" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B119" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120" s="3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121" s="3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>94</v>
+      </c>
+      <c r="B122" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>95</v>
+      </c>
+      <c r="B124" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>145</v>
+      </c>
+      <c r="B125" s="3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>153</v>
+      </c>
+      <c r="B126" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B127" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>146</v>
+      </c>
+      <c r="B128" s="3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>97</v>
+      </c>
+      <c r="B129" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>147</v>
+      </c>
+      <c r="B130" s="3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B131" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>149</v>
+      </c>
+      <c r="B133" s="3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>148</v>
+      </c>
+      <c r="B134" s="3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B136" s="3">
         <v>90</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>154</v>
+      </c>
+      <c r="B137" s="3">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2495,4 +5018,262 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B10">
+    <sortCondition ref="B1:B10"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>